<commit_message>
added GHC7 waypoint connections
</commit_message>
<xml_diff>
--- a/GHC7-waypoints.xlsx
+++ b/GHC7-waypoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsukkerd/Projects/explainable-planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E01A4B-C527-FB41-A130-BEDBA6A286CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2794D71-E494-7247-8E3E-BBF063500D4D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40200" yWindow="1040" windowWidth="28040" windowHeight="17440" xr2:uid="{450B2085-875E-6D4C-B853-5D589C4ADAD3}"/>
+    <workbookView xWindow="13180" yWindow="560" windowWidth="21320" windowHeight="16560" xr2:uid="{450B2085-875E-6D4C-B853-5D589C4ADAD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Location ID</t>
   </si>
@@ -52,6 +52,87 @@
   </si>
   <si>
     <t>Meter-to-Inch ratio</t>
+  </si>
+  <si>
+    <t>connected-to</t>
+  </si>
+  <si>
+    <t>1;3;7</t>
+  </si>
+  <si>
+    <t>2;4</t>
+  </si>
+  <si>
+    <t>3;5;9</t>
+  </si>
+  <si>
+    <t>4;10</t>
+  </si>
+  <si>
+    <t>2;6;8</t>
+  </si>
+  <si>
+    <t>7;11</t>
+  </si>
+  <si>
+    <t>4;11</t>
+  </si>
+  <si>
+    <t>5;12</t>
+  </si>
+  <si>
+    <t>8;9;12;13</t>
+  </si>
+  <si>
+    <t>10;11</t>
+  </si>
+  <si>
+    <t>11;17</t>
+  </si>
+  <si>
+    <t>14;16;19;20</t>
+  </si>
+  <si>
+    <t>15;17</t>
+  </si>
+  <si>
+    <t>13;16;18;21</t>
+  </si>
+  <si>
+    <t>17;22</t>
+  </si>
+  <si>
+    <t>15;23</t>
+  </si>
+  <si>
+    <t>17;25</t>
+  </si>
+  <si>
+    <t>18;26</t>
+  </si>
+  <si>
+    <t>19;20;24</t>
+  </si>
+  <si>
+    <t>23;27</t>
+  </si>
+  <si>
+    <t>21;26;27</t>
+  </si>
+  <si>
+    <t>22;25</t>
+  </si>
+  <si>
+    <t>27;29</t>
+  </si>
+  <si>
+    <t>28;30;31</t>
+  </si>
+  <si>
+    <t>29;32</t>
+  </si>
+  <si>
+    <t>24;25;28</t>
   </si>
 </sst>
 </file>
@@ -404,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A785292D-28EA-BB41-8A4F-1AF73CB8AC6A}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -415,11 +496,11 @@
     <col min="2" max="2" width="23.1640625" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="5" max="6" width="27.1640625" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,13 +517,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -453,21 +537,24 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="D2">
-        <f>B2+($G$1/2)</f>
+        <f>B2+($H$1/2)</f>
         <v>5.47</v>
       </c>
       <c r="E2">
-        <f>C2+($G$1/2)</f>
+        <f>C2+($H$1/2)</f>
         <v>1.1900000000000002</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -478,15 +565,18 @@
         <v>0.98</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D33" si="0">B3+($G$1/2)</f>
+        <f t="shared" ref="D3:D33" si="0">B3+($H$1/2)</f>
         <v>5.8</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E33" si="1">C3+($G$1/2)</f>
+        <f t="shared" ref="E3:E33" si="1">C3+($H$1/2)</f>
         <v>1.08</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -504,8 +594,11 @@
         <f t="shared" si="1"/>
         <v>0.94</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -523,8 +616,11 @@
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -542,8 +638,11 @@
         <f t="shared" si="1"/>
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -561,8 +660,11 @@
         <f t="shared" si="1"/>
         <v>1.6500000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -580,8 +682,11 @@
         <f t="shared" si="1"/>
         <v>1.7100000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -599,8 +704,11 @@
         <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -618,8 +726,11 @@
         <f t="shared" si="1"/>
         <v>1.26</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -637,8 +748,11 @@
         <f t="shared" si="1"/>
         <v>1.1900000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -656,8 +770,11 @@
         <f t="shared" si="1"/>
         <v>1.81</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -675,8 +792,11 @@
         <f t="shared" si="1"/>
         <v>1.81</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -694,8 +814,11 @@
         <f t="shared" si="1"/>
         <v>2.48</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -713,8 +836,11 @@
         <f t="shared" si="1"/>
         <v>3.2800000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -732,8 +858,11 @@
         <f t="shared" si="1"/>
         <v>3.2800000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -751,8 +880,11 @@
         <f t="shared" si="1"/>
         <v>3.2800000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -770,8 +902,11 @@
         <f t="shared" si="1"/>
         <v>3.2800000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -789,8 +924,11 @@
         <f t="shared" si="1"/>
         <v>3.27</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -808,8 +946,11 @@
         <f t="shared" si="1"/>
         <v>3.87</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -827,8 +968,11 @@
         <f t="shared" si="1"/>
         <v>4.07</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -846,8 +990,11 @@
         <f t="shared" si="1"/>
         <v>3.83</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -865,8 +1012,11 @@
         <f t="shared" si="1"/>
         <v>3.63</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -884,8 +1034,11 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -900,11 +1053,14 @@
         <v>6.1499999999999995</v>
       </c>
       <c r="E25">
-        <f>C25+($G$1/2)</f>
+        <f>C25+($H$1/2)</f>
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -922,8 +1078,11 @@
         <f t="shared" si="1"/>
         <v>4.2699999999999996</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -941,8 +1100,11 @@
         <f t="shared" si="1"/>
         <v>4.17</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -960,8 +1122,11 @@
         <f t="shared" si="1"/>
         <v>4.6599999999999993</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -979,8 +1144,11 @@
         <f t="shared" si="1"/>
         <v>5.4399999999999995</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -998,8 +1166,11 @@
         <f t="shared" si="1"/>
         <v>5.8999999999999995</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1017,8 +1188,11 @@
         <f t="shared" si="1"/>
         <v>6.51</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1036,8 +1210,11 @@
         <f t="shared" si="1"/>
         <v>6.08</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1054,6 +1231,9 @@
       <c r="E33">
         <f t="shared" si="1"/>
         <v>6.27</v>
+      </c>
+      <c r="F33">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>